<commit_message>
cleaning folder and adding src/
</commit_message>
<xml_diff>
--- a/output_validation/05_dimension_overview.xlsx
+++ b/output_validation/05_dimension_overview.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,253 +522,253 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>68663199</v>
+        <v>2307204</v>
       </c>
       <c r="D2" t="n">
-        <v>33</v>
+        <v>21.3</v>
       </c>
       <c r="E2" t="n">
-        <v>22642378</v>
+        <v>491129</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1</v>
+        <v>2.2</v>
       </c>
       <c r="G2" t="n">
-        <v>75499</v>
+        <v>49876</v>
       </c>
       <c r="H2" t="n">
-        <v>0.4</v>
+        <v>26.2</v>
       </c>
       <c r="I2" t="n">
-        <v>286415</v>
+        <v>603526</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9</v>
+        <v>2.9</v>
       </c>
       <c r="K2" t="n">
-        <v>598007</v>
+        <v>67720</v>
       </c>
       <c r="L2" t="n">
-        <v>65.59999999999999</v>
+        <v>47.5</v>
       </c>
       <c r="M2" t="n">
-        <v>45060900</v>
+        <v>1094955</v>
       </c>
       <c r="N2" t="n">
-        <v>34.4</v>
+        <v>52.5</v>
       </c>
       <c r="O2" t="n">
-        <v>23602299</v>
+        <v>1212250</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>non_pdi (5-17 y.o.)</t>
+          <t>hote (5-17 y.o.)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>non_pdi</t>
+          <t>hote</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>48523504</v>
+        <v>2077436</v>
       </c>
       <c r="D3" t="n">
-        <v>24.4</v>
+        <v>20.9</v>
       </c>
       <c r="E3" t="n">
-        <v>11822828</v>
+        <v>434615</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1</v>
+        <v>2.1</v>
       </c>
       <c r="G3" t="n">
-        <v>52304</v>
+        <v>43979</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5</v>
+        <v>26</v>
       </c>
       <c r="I3" t="n">
-        <v>227095</v>
+        <v>540693</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9</v>
+        <v>2.9</v>
       </c>
       <c r="K3" t="n">
-        <v>423026</v>
+        <v>59824</v>
       </c>
       <c r="L3" t="n">
-        <v>74.2</v>
+        <v>48.1</v>
       </c>
       <c r="M3" t="n">
-        <v>35998252</v>
+        <v>998326</v>
       </c>
       <c r="N3" t="n">
-        <v>25.8</v>
+        <v>51.9</v>
       </c>
       <c r="O3" t="n">
-        <v>12525253</v>
+        <v>1079110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>pdi (5-17 y.o.)</t>
+          <t>idp_host (5-17 y.o.)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>pdi</t>
+          <t>idp_host</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>20139695</v>
+        <v>125059</v>
       </c>
       <c r="D4" t="n">
-        <v>53.7</v>
+        <v>23.8</v>
       </c>
       <c r="E4" t="n">
-        <v>10819550</v>
+        <v>29787</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
-        <v>23195</v>
+        <v>2561</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3</v>
+        <v>24.7</v>
       </c>
       <c r="I4" t="n">
-        <v>59320</v>
+        <v>30925</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9</v>
+        <v>2.8</v>
       </c>
       <c r="K4" t="n">
-        <v>174981</v>
+        <v>3476</v>
       </c>
       <c r="L4" t="n">
-        <v>45</v>
+        <v>46.6</v>
       </c>
       <c r="M4" t="n">
-        <v>9062649</v>
+        <v>58310</v>
       </c>
       <c r="N4" t="n">
-        <v>55</v>
+        <v>53.4</v>
       </c>
       <c r="O4" t="n">
-        <v>11077047</v>
+        <v>66749</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Filles (5-17 ans)</t>
+          <t>retourne (5-17 y.o.)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tous les groupes de population</t>
+          <t>retourne</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>30193399</v>
+        <v>77546</v>
       </c>
       <c r="D5" t="n">
-        <v>34.1</v>
+        <v>24.3</v>
       </c>
       <c r="E5" t="n">
-        <v>10282418</v>
+        <v>18874</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1</v>
+        <v>3.4</v>
       </c>
       <c r="G5" t="n">
-        <v>15539</v>
+        <v>2658</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4</v>
+        <v>31.4</v>
       </c>
       <c r="I5" t="n">
-        <v>106744</v>
+        <v>24380</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8</v>
+        <v>4.5</v>
       </c>
       <c r="K5" t="n">
-        <v>243257</v>
+        <v>3509</v>
       </c>
       <c r="L5" t="n">
-        <v>64.7</v>
+        <v>36.3</v>
       </c>
       <c r="M5" t="n">
-        <v>19545441</v>
+        <v>28124</v>
       </c>
       <c r="N5" t="n">
-        <v>35.3</v>
+        <v>63.7</v>
       </c>
       <c r="O5" t="n">
-        <v>10647958</v>
+        <v>49422</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Garcons (5-17 ans)</t>
+          <t>idp_site (5-17 y.o.)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tous les groupes de population</t>
+          <t>idp_site</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>38469800</v>
+        <v>27164</v>
       </c>
       <c r="D6" t="n">
-        <v>31.8</v>
+        <v>28.9</v>
       </c>
       <c r="E6" t="n">
-        <v>12247982</v>
+        <v>7853</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2</v>
+        <v>2.5</v>
       </c>
       <c r="G6" t="n">
-        <v>62081</v>
+        <v>678</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5</v>
+        <v>27.7</v>
       </c>
       <c r="I6" t="n">
-        <v>190004</v>
+        <v>7528</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9</v>
+        <v>3.4</v>
       </c>
       <c r="K6" t="n">
-        <v>355336</v>
+        <v>911</v>
       </c>
       <c r="L6" t="n">
-        <v>66.59999999999999</v>
+        <v>37.5</v>
       </c>
       <c r="M6" t="n">
-        <v>25614397</v>
+        <v>10195</v>
       </c>
       <c r="N6" t="n">
-        <v>33.4</v>
+        <v>62.5</v>
       </c>
       <c r="O6" t="n">
-        <v>12855403</v>
+        <v>16970</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Éducation préscolaire (5 ans)</t>
+          <t>Filles (5-17 ans)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -777,49 +777,49 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6978393</v>
+        <v>1176674</v>
       </c>
       <c r="D7" t="n">
-        <v>63.3</v>
+        <v>22.4</v>
       </c>
       <c r="E7" t="n">
-        <v>4420486</v>
+        <v>263952</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1</v>
+        <v>2.4</v>
       </c>
       <c r="G7" t="n">
-        <v>5418</v>
+        <v>28789</v>
       </c>
       <c r="H7" t="n">
-        <v>0.4</v>
+        <v>26</v>
       </c>
       <c r="I7" t="n">
-        <v>29389</v>
+        <v>306362</v>
       </c>
       <c r="J7" t="n">
-        <v>0.5</v>
+        <v>2.9</v>
       </c>
       <c r="K7" t="n">
-        <v>32932</v>
+        <v>34418</v>
       </c>
       <c r="L7" t="n">
-        <v>35.7</v>
+        <v>46.2</v>
       </c>
       <c r="M7" t="n">
-        <v>2490167</v>
+        <v>543153</v>
       </c>
       <c r="N7" t="n">
-        <v>64.3</v>
+        <v>53.8</v>
       </c>
       <c r="O7" t="n">
-        <v>4488226</v>
+        <v>633521</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>École primaire</t>
+          <t>Garcons (5-17 ans)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -828,49 +828,49 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>26408923</v>
+        <v>1129288</v>
       </c>
       <c r="D8" t="n">
-        <v>22.4</v>
+        <v>20.2</v>
       </c>
       <c r="E8" t="n">
-        <v>5914019</v>
+        <v>228254</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="G8" t="n">
-        <v>10888</v>
+        <v>21528</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4</v>
+        <v>26.2</v>
       </c>
       <c r="I8" t="n">
-        <v>97051</v>
+        <v>295484</v>
       </c>
       <c r="J8" t="n">
-        <v>1.1</v>
+        <v>2.9</v>
       </c>
       <c r="K8" t="n">
-        <v>299759</v>
+        <v>33235</v>
       </c>
       <c r="L8" t="n">
-        <v>76.09999999999999</v>
+        <v>48.8</v>
       </c>
       <c r="M8" t="n">
-        <v>20087206</v>
+        <v>550787</v>
       </c>
       <c r="N8" t="n">
-        <v>23.9</v>
+        <v>51.2</v>
       </c>
       <c r="O8" t="n">
-        <v>6321717</v>
+        <v>578500</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Niveau scolaire intermédiaire</t>
+          <t>Éducation préscolaire (5 ans)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -879,94 +879,196 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>21127138</v>
+        <v>134153</v>
       </c>
       <c r="D9" t="n">
-        <v>31</v>
+        <v>53.3</v>
       </c>
       <c r="E9" t="n">
-        <v>6555234</v>
+        <v>71504</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2</v>
+        <v>3.7</v>
       </c>
       <c r="G9" t="n">
-        <v>33804</v>
+        <v>4967</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5</v>
+        <v>11.9</v>
       </c>
       <c r="I9" t="n">
-        <v>99615</v>
+        <v>15922</v>
       </c>
       <c r="J9" t="n">
-        <v>0.9</v>
+        <v>1.5</v>
       </c>
       <c r="K9" t="n">
-        <v>188863</v>
+        <v>1948</v>
       </c>
       <c r="L9" t="n">
-        <v>67.40000000000001</v>
+        <v>29.7</v>
       </c>
       <c r="M9" t="n">
-        <v>14249623</v>
+        <v>39813</v>
       </c>
       <c r="N9" t="n">
-        <v>32.6</v>
+        <v>70.3</v>
       </c>
       <c r="O9" t="n">
-        <v>6877515</v>
+        <v>94340</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>École primaire</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Tous les groupes de population</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1242341</v>
+      </c>
+      <c r="D10" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>252799</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>18596</v>
+      </c>
+      <c r="H10" t="n">
+        <v>26.7</v>
+      </c>
+      <c r="I10" t="n">
+        <v>331596</v>
+      </c>
+      <c r="J10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K10" t="n">
+        <v>36994</v>
+      </c>
+      <c r="L10" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="M10" t="n">
+        <v>602355</v>
+      </c>
+      <c r="N10" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="O10" t="n">
+        <v>639986</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Niveau scolaire intermédiaire</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Tous les groupes de population</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>709129</v>
+      </c>
+      <c r="D11" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>123654</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G11" t="n">
+        <v>18254</v>
+      </c>
+      <c r="H11" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="I11" t="n">
+        <v>190763</v>
+      </c>
+      <c r="J11" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="K11" t="n">
+        <v>20858</v>
+      </c>
+      <c r="L11" t="n">
+        <v>50.1</v>
+      </c>
+      <c r="M11" t="n">
+        <v>355600</v>
+      </c>
+      <c r="N11" t="n">
+        <v>49.9</v>
+      </c>
+      <c r="O11" t="n">
+        <v>353529</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>École secondaire</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Tous les groupes de population</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>15845354</v>
-      </c>
-      <c r="D10" t="n">
-        <v>49.5</v>
-      </c>
-      <c r="E10" t="n">
-        <v>7851209</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G10" t="n">
-        <v>31752</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I10" t="n">
-        <v>71926</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="K10" t="n">
-        <v>44492</v>
-      </c>
-      <c r="L10" t="n">
-        <v>49.5</v>
-      </c>
-      <c r="M10" t="n">
-        <v>7845974</v>
-      </c>
-      <c r="N10" t="n">
-        <v>50.5</v>
-      </c>
-      <c r="O10" t="n">
-        <v>7999380</v>
+      <c r="C12" t="n">
+        <v>175507</v>
+      </c>
+      <c r="D12" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>34056</v>
+      </c>
+      <c r="F12" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="G12" t="n">
+        <v>9890</v>
+      </c>
+      <c r="H12" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>45991</v>
+      </c>
+      <c r="J12" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K12" t="n">
+        <v>7850</v>
+      </c>
+      <c r="L12" t="n">
+        <v>44.3</v>
+      </c>
+      <c r="M12" t="n">
+        <v>77721</v>
+      </c>
+      <c r="N12" t="n">
+        <v>55.7</v>
+      </c>
+      <c r="O12" t="n">
+        <v>97786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>